<commit_message>
se der erro nesse grafo de novo eu me m
</commit_message>
<xml_diff>
--- a/project/Anexo/critical_path/TOY.xlsx
+++ b/project/Anexo/critical_path/TOY.xlsx
@@ -5,22 +5,30 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\George\Professor\Ensino\Graduacao\CSI105 Algoritmos e Estruturas de Dados III\Trabalhos\2022-2\Trabalho 2\Tarefa\Anexo\critical_path\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\George\Professor\Ensino\Graduacao\CSI466 Teoria dos Grafos\Trabalhos\2022-2\Trabalho 2\Tarefa\Anexo\critical_path\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC9CE193-4E83-4F46-92AA-3517F1D2DB0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3339E5-665A-486E-9199-771F3849040D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Página1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Código</t>
   </si>
@@ -83,6 +91,9 @@
   </si>
   <si>
     <t>Duração</t>
+  </si>
+  <si>
+    <t>CS001;CS004</t>
   </si>
 </sst>
 </file>
@@ -353,7 +364,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -451,7 +462,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>